<commit_message>
Update DogBoneSDRAMv1 (version 1).xlsb.xlsx
With whatever may have changed in it
</commit_message>
<xml_diff>
--- a/docs/DogBoneSDRAMv1 (version 1).xlsb.xlsx
+++ b/docs/DogBoneSDRAMv1 (version 1).xlsb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\EVKB_1060\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D13EE1-4F72-4570-8DF6-8B6C37039014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{224BE540-40CD-438C-AE6F-F4A3BDAB8292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="2460" windowWidth="27690" windowHeight="18345" tabRatio="400" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10665" yWindow="2535" windowWidth="26370" windowHeight="16965" tabRatio="400" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2044" uniqueCount="1082">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2046" uniqueCount="1084">
   <si>
     <t>B0_01</t>
   </si>
@@ -3496,6 +3496,12 @@
   </si>
   <si>
     <t>WDOG1_WDOG_RST_B_DEB</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
@@ -3644,7 +3650,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3750,6 +3756,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFCCFF33"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39994506668294322"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4289,7 +4301,6 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="12" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -4322,6 +4333,8 @@
     <xf numFmtId="20" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4331,7 +4344,6 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5168,7 +5180,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O66"/>
   <sheetViews>
-    <sheetView topLeftCell="A80" workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
@@ -9390,21 +9402,21 @@
       <c r="M10" s="96"/>
     </row>
     <row r="11" spans="1:13">
-      <c r="A11" s="143" t="s">
+      <c r="A11" s="144" t="s">
         <v>263</v>
       </c>
-      <c r="B11" s="144"/>
-      <c r="C11" s="144"/>
-      <c r="D11" s="144"/>
-      <c r="E11" s="144"/>
-      <c r="F11" s="144"/>
-      <c r="G11" s="144"/>
-      <c r="H11" s="144"/>
-      <c r="I11" s="144"/>
-      <c r="J11" s="144"/>
-      <c r="K11" s="144"/>
-      <c r="L11" s="144"/>
-      <c r="M11" s="145"/>
+      <c r="B11" s="145"/>
+      <c r="C11" s="145"/>
+      <c r="D11" s="145"/>
+      <c r="E11" s="145"/>
+      <c r="F11" s="145"/>
+      <c r="G11" s="145"/>
+      <c r="H11" s="145"/>
+      <c r="I11" s="145"/>
+      <c r="J11" s="145"/>
+      <c r="K11" s="145"/>
+      <c r="L11" s="145"/>
+      <c r="M11" s="146"/>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="86" t="s">
@@ -9540,8 +9552,8 @@
   </sheetPr>
   <dimension ref="A2:L104"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="B102" sqref="B102"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="A80" sqref="A80:L81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9610,16 +9622,16 @@
       <c r="D3" s="118" t="s">
         <v>506</v>
       </c>
-      <c r="E3" s="123" t="s">
+      <c r="E3" s="122" t="s">
         <v>757</v>
       </c>
-      <c r="F3" s="120" t="s">
+      <c r="F3" s="143" t="s">
         <v>758</v>
       </c>
-      <c r="G3" s="121" t="s">
+      <c r="G3" s="120" t="s">
         <v>760</v>
       </c>
-      <c r="H3" s="122" t="s">
+      <c r="H3" s="121" t="s">
         <v>764</v>
       </c>
       <c r="I3" s="117"/>
@@ -9638,16 +9650,16 @@
       <c r="D4" s="118" t="s">
         <v>769</v>
       </c>
-      <c r="E4" s="123" t="s">
+      <c r="E4" s="122" t="s">
         <v>768</v>
       </c>
-      <c r="F4" s="120" t="s">
+      <c r="F4" s="143" t="s">
         <v>759</v>
       </c>
-      <c r="G4" s="121" t="s">
+      <c r="G4" s="120" t="s">
         <v>761</v>
       </c>
-      <c r="H4" s="122" t="s">
+      <c r="H4" s="121" t="s">
         <v>765</v>
       </c>
       <c r="I4" s="117"/>
@@ -9666,16 +9678,16 @@
       <c r="D5" s="118" t="s">
         <v>512</v>
       </c>
-      <c r="E5" s="123" t="s">
+      <c r="E5" s="122" t="s">
         <v>770</v>
       </c>
-      <c r="F5" s="120" t="s">
+      <c r="F5" s="143" t="s">
         <v>632</v>
       </c>
-      <c r="G5" s="121" t="s">
+      <c r="G5" s="120" t="s">
         <v>762</v>
       </c>
-      <c r="H5" s="122" t="s">
+      <c r="H5" s="121" t="s">
         <v>766</v>
       </c>
       <c r="I5" s="117"/>
@@ -9694,16 +9706,16 @@
       <c r="D6" s="118" t="s">
         <v>771</v>
       </c>
-      <c r="E6" s="123" t="s">
+      <c r="E6" s="122" t="s">
         <v>772</v>
       </c>
-      <c r="F6" s="120" t="s">
+      <c r="F6" s="143" t="s">
         <v>622</v>
       </c>
-      <c r="G6" s="121" t="s">
+      <c r="G6" s="120" t="s">
         <v>763</v>
       </c>
-      <c r="H6" s="122" t="s">
+      <c r="H6" s="121" t="s">
         <v>767</v>
       </c>
       <c r="I6" s="117"/>
@@ -9725,13 +9737,13 @@
       <c r="E7" s="119" t="s">
         <v>345</v>
       </c>
-      <c r="F7" s="120" t="s">
+      <c r="F7" s="143" t="s">
         <v>346</v>
       </c>
-      <c r="G7" s="121" t="s">
+      <c r="G7" s="120" t="s">
         <v>347</v>
       </c>
-      <c r="H7" s="122" t="s">
+      <c r="H7" s="121" t="s">
         <v>348</v>
       </c>
       <c r="I7" s="117"/>
@@ -9755,7 +9767,7 @@
       <c r="E8" s="113" t="s">
         <v>352</v>
       </c>
-      <c r="F8" s="108" t="s">
+      <c r="F8" s="143" t="s">
         <v>353</v>
       </c>
       <c r="G8" s="114" t="s">
@@ -9781,7 +9793,7 @@
       <c r="E9" s="113" t="s">
         <v>359</v>
       </c>
-      <c r="F9" s="108" t="s">
+      <c r="F9" s="143" t="s">
         <v>360</v>
       </c>
       <c r="G9" s="114" t="s">
@@ -9807,7 +9819,7 @@
       <c r="E10" s="113" t="s">
         <v>598</v>
       </c>
-      <c r="F10" s="108" t="s">
+      <c r="F10" s="143" t="s">
         <v>599</v>
       </c>
       <c r="G10" s="114" t="s">
@@ -9833,7 +9845,7 @@
       <c r="E11" s="113" t="s">
         <v>366</v>
       </c>
-      <c r="F11" s="108" t="s">
+      <c r="F11" s="143" t="s">
         <v>327</v>
       </c>
       <c r="G11" s="114" t="s">
@@ -9940,7 +9952,7 @@
       <c r="C15" s="10" t="s">
         <v>793</v>
       </c>
-      <c r="D15" s="108" t="s">
+      <c r="D15" s="143" t="s">
         <v>807</v>
       </c>
       <c r="E15" s="113" t="s">
@@ -9949,7 +9961,7 @@
       <c r="F15" s="108" t="s">
         <v>583</v>
       </c>
-      <c r="G15" s="124" t="s">
+      <c r="G15" s="123" t="s">
         <v>392</v>
       </c>
       <c r="H15" s="111" t="s">
@@ -9969,7 +9981,7 @@
       <c r="C16" s="10" t="s">
         <v>794</v>
       </c>
-      <c r="D16" s="108" t="s">
+      <c r="D16" s="143" t="s">
         <v>818</v>
       </c>
       <c r="E16" s="109" t="s">
@@ -9978,7 +9990,7 @@
       <c r="F16" s="108" t="s">
         <v>405</v>
       </c>
-      <c r="G16" s="124" t="s">
+      <c r="G16" s="123" t="s">
         <v>383</v>
       </c>
       <c r="H16" s="111" t="s">
@@ -9998,7 +10010,7 @@
       <c r="C17" s="10" t="s">
         <v>795</v>
       </c>
-      <c r="D17" s="108" t="s">
+      <c r="D17" s="143" t="s">
         <v>821</v>
       </c>
       <c r="E17" s="109" t="s">
@@ -10027,7 +10039,7 @@
       <c r="C18" s="10" t="s">
         <v>796</v>
       </c>
-      <c r="D18" s="108" t="s">
+      <c r="D18" s="143" t="s">
         <v>824</v>
       </c>
       <c r="E18" s="109" t="s">
@@ -10056,7 +10068,7 @@
       <c r="C19" s="10" t="s">
         <v>797</v>
       </c>
-      <c r="D19" s="108" t="s">
+      <c r="D19" s="143" t="s">
         <v>825</v>
       </c>
       <c r="E19" s="109" t="s">
@@ -10462,7 +10474,7 @@
       <c r="F33" s="112" t="s">
         <v>623</v>
       </c>
-      <c r="G33" s="128" t="s">
+      <c r="G33" s="127" t="s">
         <v>857</v>
       </c>
       <c r="H33" s="111" t="s">
@@ -10491,7 +10503,7 @@
       <c r="F34" s="10" t="s">
         <v>563</v>
       </c>
-      <c r="G34" s="128" t="s">
+      <c r="G34" s="127" t="s">
         <v>564</v>
       </c>
       <c r="H34" s="111" t="s">
@@ -10520,7 +10532,7 @@
       <c r="F35" s="10" t="s">
         <v>555</v>
       </c>
-      <c r="G35" s="128" t="s">
+      <c r="G35" s="127" t="s">
         <v>556</v>
       </c>
       <c r="H35" s="111" t="s">
@@ -10549,7 +10561,7 @@
       <c r="F36" s="10" t="s">
         <v>870</v>
       </c>
-      <c r="G36" s="128" t="s">
+      <c r="G36" s="127" t="s">
         <v>871</v>
       </c>
       <c r="H36" s="111" t="s">
@@ -10581,7 +10593,7 @@
       <c r="F37" s="10" t="s">
         <v>875</v>
       </c>
-      <c r="G37" s="128" t="s">
+      <c r="G37" s="127" t="s">
         <v>872</v>
       </c>
       <c r="H37" s="111" t="s">
@@ -10610,7 +10622,7 @@
       <c r="F38" s="10" t="s">
         <v>878</v>
       </c>
-      <c r="G38" s="128" t="s">
+      <c r="G38" s="127" t="s">
         <v>873</v>
       </c>
       <c r="H38" s="111" t="s">
@@ -10633,7 +10645,7 @@
       <c r="C39" s="10" t="s">
         <v>577</v>
       </c>
-      <c r="D39" s="108" t="s">
+      <c r="D39" s="143" t="s">
         <v>578</v>
       </c>
       <c r="E39" s="10" t="s">
@@ -10642,7 +10654,7 @@
       <c r="F39" s="10" t="s">
         <v>580</v>
       </c>
-      <c r="G39" s="128" t="s">
+      <c r="G39" s="127" t="s">
         <v>581</v>
       </c>
       <c r="H39" s="111" t="s">
@@ -10668,7 +10680,7 @@
       <c r="C40" s="10" t="s">
         <v>568</v>
       </c>
-      <c r="D40" s="108" t="s">
+      <c r="D40" s="143" t="s">
         <v>569</v>
       </c>
       <c r="E40" s="10" t="s">
@@ -10677,7 +10689,7 @@
       <c r="F40" s="10" t="s">
         <v>571</v>
       </c>
-      <c r="G40" s="128" t="s">
+      <c r="G40" s="127" t="s">
         <v>572</v>
       </c>
       <c r="H40" s="111" t="s">
@@ -10712,7 +10724,7 @@
       <c r="F41" s="10" t="s">
         <v>884</v>
       </c>
-      <c r="G41" s="128" t="s">
+      <c r="G41" s="127" t="s">
         <v>885</v>
       </c>
       <c r="H41" s="111" t="s">
@@ -10831,7 +10843,7 @@
       <c r="C45" s="10" t="s">
         <v>326</v>
       </c>
-      <c r="D45" s="108" t="s">
+      <c r="D45" s="143" t="s">
         <v>327</v>
       </c>
       <c r="E45" s="109" t="s">
@@ -10863,7 +10875,7 @@
       <c r="C46" s="10" t="s">
         <v>334</v>
       </c>
-      <c r="D46" s="108" t="s">
+      <c r="D46" s="143" t="s">
         <v>335</v>
       </c>
       <c r="E46" s="109" t="s">
@@ -10892,7 +10904,7 @@
       <c r="B47" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C47" s="127" t="s">
+      <c r="C47" s="126" t="s">
         <v>369</v>
       </c>
       <c r="D47" s="110" t="s">
@@ -10924,10 +10936,10 @@
       <c r="B48" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C48" s="127" t="s">
+      <c r="C48" s="126" t="s">
         <v>377</v>
       </c>
-      <c r="D48" s="108" t="s">
+      <c r="D48" s="143" t="s">
         <v>378</v>
       </c>
       <c r="E48" s="109" t="s">
@@ -10959,10 +10971,10 @@
       <c r="B49" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C49" s="127" t="s">
+      <c r="C49" s="126" t="s">
         <v>386</v>
       </c>
-      <c r="D49" s="108" t="s">
+      <c r="D49" s="143" t="s">
         <v>387</v>
       </c>
       <c r="E49" s="109" t="s">
@@ -10994,7 +11006,7 @@
       <c r="B50" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C50" s="127" t="s">
+      <c r="C50" s="126" t="s">
         <v>395</v>
       </c>
       <c r="D50" s="110" t="s">
@@ -11026,7 +11038,7 @@
       <c r="B51" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="C51" s="127" t="s">
+      <c r="C51" s="126" t="s">
         <v>314</v>
       </c>
       <c r="D51" s="110" t="s">
@@ -11058,7 +11070,7 @@
       <c r="B52" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C52" s="127" t="s">
+      <c r="C52" s="126" t="s">
         <v>315</v>
       </c>
       <c r="D52" s="110" t="s">
@@ -11090,7 +11102,7 @@
       <c r="B53" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C53" s="127" t="s">
+      <c r="C53" s="126" t="s">
         <v>212</v>
       </c>
       <c r="D53" s="110" t="s">
@@ -11122,7 +11134,7 @@
       <c r="B54" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C54" s="127" t="s">
+      <c r="C54" s="126" t="s">
         <v>306</v>
       </c>
       <c r="D54" s="110" t="s">
@@ -11242,7 +11254,7 @@
       <c r="F57" s="10" t="s">
         <v>456</v>
       </c>
-      <c r="G57" s="128" t="s">
+      <c r="G57" s="127" t="s">
         <v>223</v>
       </c>
       <c r="H57" s="111" t="s">
@@ -11280,7 +11292,7 @@
       <c r="F58" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="G58" s="128" t="s">
+      <c r="G58" s="127" t="s">
         <v>76</v>
       </c>
       <c r="H58" s="111" t="s">
@@ -11394,7 +11406,7 @@
       <c r="F61" s="113" t="s">
         <v>488</v>
       </c>
-      <c r="G61" s="128" t="s">
+      <c r="G61" s="127" t="s">
         <v>489</v>
       </c>
       <c r="H61" s="111" t="s">
@@ -11432,7 +11444,7 @@
       <c r="F62" s="113" t="s">
         <v>498</v>
       </c>
-      <c r="G62" s="128" t="s">
+      <c r="G62" s="127" t="s">
         <v>499</v>
       </c>
       <c r="H62" s="111" t="s">
@@ -11470,7 +11482,7 @@
       <c r="F63" s="10" t="s">
         <v>472</v>
       </c>
-      <c r="G63" s="128" t="s">
+      <c r="G63" s="127" t="s">
         <v>507</v>
       </c>
       <c r="H63" s="111" t="s">
@@ -11505,7 +11517,7 @@
       <c r="F64" s="113" t="s">
         <v>513</v>
       </c>
-      <c r="G64" s="128" t="s">
+      <c r="G64" s="127" t="s">
         <v>514</v>
       </c>
       <c r="H64" s="111" t="s">
@@ -11604,7 +11616,7 @@
       <c r="F67" s="10" t="s">
         <v>534</v>
       </c>
-      <c r="G67" s="146" t="s">
+      <c r="G67" s="142" t="s">
         <v>535</v>
       </c>
       <c r="H67" s="111" t="s">
@@ -11642,7 +11654,7 @@
       <c r="F68" s="10" t="s">
         <v>544</v>
       </c>
-      <c r="G68" s="128" t="s">
+      <c r="G68" s="127" t="s">
         <v>545</v>
       </c>
       <c r="H68" s="111" t="s">
@@ -11668,10 +11680,10 @@
       <c r="B69" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C69" s="127" t="s">
+      <c r="C69" s="126" t="s">
         <v>587</v>
       </c>
-      <c r="D69" s="108" t="s">
+      <c r="D69" s="143" t="s">
         <v>588</v>
       </c>
       <c r="E69" s="10" t="s">
@@ -11694,7 +11706,7 @@
       </c>
     </row>
     <row r="70" spans="1:12">
-      <c r="A70" s="126" t="s">
+      <c r="A70" s="125" t="s">
         <v>602</v>
       </c>
       <c r="B70" s="10" t="s">
@@ -11709,7 +11721,7 @@
       <c r="E70" s="109" t="s">
         <v>606</v>
       </c>
-      <c r="F70" s="108" t="s">
+      <c r="F70" s="143" t="s">
         <v>353</v>
       </c>
       <c r="G70" s="112" t="s">
@@ -11726,7 +11738,7 @@
       </c>
     </row>
     <row r="71" spans="1:12">
-      <c r="A71" s="126" t="s">
+      <c r="A71" s="125" t="s">
         <v>610</v>
       </c>
       <c r="B71" s="10" t="s">
@@ -11741,7 +11753,7 @@
       <c r="E71" s="109" t="s">
         <v>614</v>
       </c>
-      <c r="F71" s="108" t="s">
+      <c r="F71" s="143" t="s">
         <v>346</v>
       </c>
       <c r="G71" s="112" t="s">
@@ -11758,7 +11770,7 @@
       </c>
     </row>
     <row r="72" spans="1:12">
-      <c r="A72" s="126" t="s">
+      <c r="A72" s="125" t="s">
         <v>618</v>
       </c>
       <c r="B72" s="10" t="s">
@@ -11773,7 +11785,7 @@
       <c r="E72" s="116" t="s">
         <v>462</v>
       </c>
-      <c r="F72" s="108" t="s">
+      <c r="F72" s="143" t="s">
         <v>622</v>
       </c>
       <c r="G72" s="112" t="s">
@@ -11793,7 +11805,7 @@
       </c>
     </row>
     <row r="73" spans="1:12">
-      <c r="A73" s="126" t="s">
+      <c r="A73" s="125" t="s">
         <v>628</v>
       </c>
       <c r="B73" s="10" t="s">
@@ -11808,7 +11820,7 @@
       <c r="E73" s="116" t="s">
         <v>454</v>
       </c>
-      <c r="F73" s="108" t="s">
+      <c r="F73" s="143" t="s">
         <v>632</v>
       </c>
       <c r="G73" s="112" t="s">
@@ -11828,7 +11840,7 @@
       </c>
     </row>
     <row r="74" spans="1:12">
-      <c r="A74" s="126" t="s">
+      <c r="A74" s="125" t="s">
         <v>636</v>
       </c>
       <c r="B74" s="10" t="s">
@@ -11843,7 +11855,7 @@
       <c r="E74" s="109" t="s">
         <v>487</v>
       </c>
-      <c r="F74" s="108" t="s">
+      <c r="F74" s="143" t="s">
         <v>360</v>
       </c>
       <c r="G74" s="10" t="s">
@@ -11860,7 +11872,7 @@
       </c>
     </row>
     <row r="75" spans="1:12">
-      <c r="A75" s="126" t="s">
+      <c r="A75" s="125" t="s">
         <v>643</v>
       </c>
       <c r="B75" s="10" t="s">
@@ -11875,7 +11887,7 @@
       <c r="E75" s="109" t="s">
         <v>497</v>
       </c>
-      <c r="F75" s="108" t="s">
+      <c r="F75" s="143" t="s">
         <v>599</v>
       </c>
       <c r="G75" s="10" t="s">
@@ -11898,7 +11910,7 @@
       <c r="B76" t="s">
         <v>3</v>
       </c>
-      <c r="C76" s="127" t="s">
+      <c r="C76" s="126" t="s">
         <v>651</v>
       </c>
       <c r="D76" s="110" t="s">
@@ -11930,7 +11942,7 @@
       <c r="B77" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C77" s="127" t="s">
+      <c r="C77" s="126" t="s">
         <v>660</v>
       </c>
       <c r="D77" s="110" t="s">
@@ -11962,7 +11974,7 @@
       <c r="B78" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C78" s="127" t="s">
+      <c r="C78" s="126" t="s">
         <v>669</v>
       </c>
       <c r="D78" s="110" t="s">
@@ -11994,7 +12006,7 @@
       <c r="B79" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C79" s="127" t="s">
+      <c r="C79" s="126" t="s">
         <v>676</v>
       </c>
       <c r="D79" s="110" t="s">
@@ -12026,7 +12038,7 @@
       <c r="B80" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C80" s="127" t="s">
+      <c r="C80" s="126" t="s">
         <v>684</v>
       </c>
       <c r="D80" s="110" t="s">
@@ -12058,7 +12070,7 @@
       <c r="B81" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C81" s="127" t="s">
+      <c r="C81" s="126" t="s">
         <v>690</v>
       </c>
       <c r="D81" s="110" t="s">
@@ -12084,563 +12096,563 @@
       </c>
     </row>
     <row r="82" spans="1:12">
-      <c r="A82" s="125" t="s">
+      <c r="A82" s="10" t="s">
         <v>913</v>
       </c>
       <c r="B82" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C82" s="126" t="s">
+        <v>909</v>
+      </c>
+      <c r="D82" s="143" t="s">
+        <v>914</v>
+      </c>
+      <c r="E82" s="10" t="s">
+        <v>915</v>
+      </c>
+      <c r="F82" s="113" t="s">
+        <v>513</v>
+      </c>
+      <c r="G82" s="114" t="s">
+        <v>916</v>
+      </c>
+      <c r="H82" s="111" t="s">
+        <v>919</v>
+      </c>
+      <c r="I82" s="10" t="s">
+        <v>922</v>
+      </c>
+      <c r="K82" s="10" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12">
+      <c r="A83" s="124" t="s">
+        <v>705</v>
+      </c>
+      <c r="B83" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C82" s="127" t="s">
+      <c r="C83" s="126" t="s">
         <v>910</v>
       </c>
-      <c r="D82" s="108" t="s">
+      <c r="D83" s="143" t="s">
         <v>924</v>
       </c>
-      <c r="E82" s="10" t="s">
+      <c r="E83" s="10" t="s">
         <v>926</v>
       </c>
-      <c r="F82" s="113" t="s">
+      <c r="F83" s="113" t="s">
         <v>488</v>
       </c>
-      <c r="G82" s="114" t="s">
+      <c r="G83" s="114" t="s">
         <v>917</v>
       </c>
-      <c r="H82" s="111" t="s">
+      <c r="H83" s="111" t="s">
         <v>920</v>
       </c>
-      <c r="I82" s="10" t="s">
+      <c r="I83" s="10" t="s">
         <v>927</v>
       </c>
-      <c r="K82" s="10" t="s">
+      <c r="K83" s="10" t="s">
         <v>558</v>
       </c>
     </row>
-    <row r="83" spans="1:12">
-      <c r="A83" s="125" t="s">
-        <v>705</v>
-      </c>
-      <c r="B83" s="10" t="s">
+    <row r="84" spans="1:12">
+      <c r="A84" s="124" t="s">
+        <v>727</v>
+      </c>
+      <c r="B84" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C83" s="127" t="s">
+      <c r="C84" s="126" t="s">
         <v>911</v>
       </c>
-      <c r="D83" s="108" t="s">
+      <c r="D84" s="143" t="s">
         <v>925</v>
       </c>
-      <c r="E83" s="10" t="s">
+      <c r="E84" s="10" t="s">
         <v>928</v>
       </c>
-      <c r="F83" s="113" t="s">
+      <c r="F84" s="113" t="s">
         <v>929</v>
       </c>
-      <c r="G83" s="114" t="s">
+      <c r="G84" s="114" t="s">
         <v>918</v>
       </c>
-      <c r="H83" s="111" t="s">
+      <c r="H84" s="111" t="s">
         <v>921</v>
       </c>
-      <c r="I83" s="10" t="s">
+      <c r="I84" s="10" t="s">
         <v>930</v>
       </c>
-      <c r="K83" s="10" t="s">
+      <c r="K84" s="10" t="s">
         <v>930</v>
       </c>
-      <c r="L83" s="10" t="s">
+      <c r="L84" s="10" t="s">
         <v>627</v>
       </c>
     </row>
-    <row r="84" spans="1:12">
-      <c r="A84" s="125" t="s">
-        <v>727</v>
-      </c>
-      <c r="B84" s="10" t="s">
+    <row r="85" spans="1:12">
+      <c r="A85" s="124" t="s">
+        <v>734</v>
+      </c>
+      <c r="B85" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C84" s="127" t="s">
+      <c r="C85" s="126" t="s">
         <v>939</v>
       </c>
-      <c r="D84" s="108" t="s">
+      <c r="D85" s="143" t="s">
         <v>335</v>
       </c>
-      <c r="E84" s="116" t="s">
+      <c r="E85" s="116" t="s">
         <v>949</v>
       </c>
-      <c r="F84" s="113" t="s">
+      <c r="F85" s="113" t="s">
         <v>534</v>
       </c>
-      <c r="G84" s="114" t="s">
+      <c r="G85" s="114" t="s">
         <v>950</v>
       </c>
-      <c r="H84" s="111" t="s">
+      <c r="H85" s="111" t="s">
         <v>964</v>
       </c>
-      <c r="I84" s="110" t="s">
+      <c r="I85" s="110" t="s">
         <v>838</v>
       </c>
-      <c r="K84" s="10" t="s">
+      <c r="K85" s="10" t="s">
         <v>584</v>
       </c>
-      <c r="L84" s="114" t="s">
+      <c r="L85" s="114" t="s">
         <v>980</v>
       </c>
     </row>
-    <row r="85" spans="1:12">
-      <c r="A85" s="125" t="s">
-        <v>734</v>
-      </c>
-      <c r="B85" s="10" t="s">
+    <row r="86" spans="1:12">
+      <c r="A86" s="124" t="s">
+        <v>697</v>
+      </c>
+      <c r="B86" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C85" s="127" t="s">
+      <c r="C86" s="126" t="s">
         <v>940</v>
       </c>
-      <c r="D85" s="108" t="s">
+      <c r="D86" s="143" t="s">
         <v>327</v>
       </c>
-      <c r="E85" s="116" t="s">
+      <c r="E86" s="116" t="s">
         <v>978</v>
       </c>
-      <c r="F85" s="113" t="s">
+      <c r="F86" s="113" t="s">
         <v>544</v>
       </c>
-      <c r="G85" s="114" t="s">
+      <c r="G86" s="114" t="s">
         <v>951</v>
       </c>
-      <c r="H85" s="111" t="s">
+      <c r="H86" s="111" t="s">
         <v>965</v>
       </c>
-      <c r="I85" s="110" t="s">
+      <c r="I86" s="110" t="s">
         <v>979</v>
       </c>
-      <c r="K85" s="10" t="s">
+      <c r="K86" s="10" t="s">
         <v>574</v>
       </c>
-      <c r="L85" s="114" t="s">
+      <c r="L86" s="114" t="s">
         <v>981</v>
       </c>
     </row>
-    <row r="86" spans="1:12">
-      <c r="A86" s="125" t="s">
-        <v>697</v>
-      </c>
-      <c r="B86" s="10" t="s">
+    <row r="87" spans="1:12">
+      <c r="A87" s="124" t="s">
+        <v>720</v>
+      </c>
+      <c r="B87" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C86" s="127" t="s">
+      <c r="C87" s="126" t="s">
         <v>941</v>
       </c>
-      <c r="D86" s="108" t="s">
+      <c r="D87" s="108" t="s">
         <v>406</v>
       </c>
-      <c r="E86" s="128" t="s">
+      <c r="E87" s="127" t="s">
         <v>982</v>
       </c>
-      <c r="F86" s="113" t="s">
+      <c r="F87" s="113" t="s">
         <v>983</v>
       </c>
-      <c r="G86" s="114" t="s">
+      <c r="G87" s="114" t="s">
         <v>952</v>
       </c>
-      <c r="H86" s="111" t="s">
+      <c r="H87" s="111" t="s">
         <v>966</v>
       </c>
-      <c r="K86" s="10" t="s">
+      <c r="K87" s="10" t="s">
         <v>984</v>
       </c>
-      <c r="L86" s="114" t="s">
+      <c r="L87" s="114" t="s">
         <v>985</v>
       </c>
     </row>
-    <row r="87" spans="1:12">
-      <c r="A87" s="125" t="s">
-        <v>720</v>
-      </c>
-      <c r="B87" s="10" t="s">
+    <row r="88" spans="1:12">
+      <c r="A88" s="124" t="s">
+        <v>713</v>
+      </c>
+      <c r="B88" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C87" s="127" t="s">
+      <c r="C88" s="126" t="s">
         <v>942</v>
       </c>
-      <c r="D87" s="108" t="s">
+      <c r="D88" s="108" t="s">
         <v>421</v>
       </c>
-      <c r="E87" s="128" t="s">
+      <c r="E88" s="127" t="s">
         <v>986</v>
       </c>
-      <c r="F87" s="113" t="s">
+      <c r="F88" s="113" t="s">
         <v>987</v>
       </c>
-      <c r="G87" s="114" t="s">
+      <c r="G88" s="114" t="s">
         <v>953</v>
       </c>
-      <c r="H87" s="111" t="s">
+      <c r="H88" s="111" t="s">
         <v>967</v>
       </c>
-      <c r="K87" s="10" t="s">
+      <c r="K88" s="10" t="s">
         <v>988</v>
       </c>
-      <c r="L87" s="114" t="s">
+      <c r="L88" s="114" t="s">
         <v>989</v>
       </c>
     </row>
-    <row r="88" spans="1:12">
-      <c r="A88" s="125" t="s">
-        <v>713</v>
-      </c>
-      <c r="B88" s="10" t="s">
+    <row r="89" spans="1:12">
+      <c r="A89" s="124" t="s">
+        <v>741</v>
+      </c>
+      <c r="B89" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C88" s="127" t="s">
+      <c r="C89" s="126" t="s">
         <v>943</v>
       </c>
-      <c r="D88" s="108" t="s">
+      <c r="D89" s="108" t="s">
         <v>414</v>
       </c>
-      <c r="E88" s="128" t="s">
+      <c r="E89" s="127" t="s">
         <v>990</v>
       </c>
-      <c r="F88" s="113" t="s">
+      <c r="F89" s="113" t="s">
         <v>849</v>
       </c>
-      <c r="G88" s="114" t="s">
+      <c r="G89" s="114" t="s">
         <v>954</v>
       </c>
-      <c r="H88" s="111" t="s">
+      <c r="H89" s="111" t="s">
         <v>968</v>
       </c>
-      <c r="K88" s="10" t="s">
+      <c r="K89" s="10" t="s">
         <v>850</v>
       </c>
-      <c r="L88" s="114" t="s">
+      <c r="L89" s="114" t="s">
         <v>991</v>
       </c>
     </row>
-    <row r="89" spans="1:12">
-      <c r="A89" s="125" t="s">
-        <v>741</v>
-      </c>
-      <c r="B89" s="10" t="s">
+    <row r="90" spans="1:12">
+      <c r="A90" s="124" t="s">
+        <v>931</v>
+      </c>
+      <c r="B90" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C89" s="127" t="s">
+      <c r="C90" s="126" t="s">
         <v>944</v>
       </c>
-      <c r="D89" s="108" t="s">
+      <c r="D90" s="108" t="s">
         <v>429</v>
       </c>
-      <c r="E89" s="128" t="s">
+      <c r="E90" s="127" t="s">
         <v>995</v>
       </c>
-      <c r="F89" s="113" t="s">
+      <c r="F90" s="113" t="s">
         <v>992</v>
       </c>
-      <c r="G89" s="114" t="s">
+      <c r="G90" s="114" t="s">
         <v>955</v>
       </c>
-      <c r="H89" s="111" t="s">
+      <c r="H90" s="111" t="s">
         <v>969</v>
       </c>
-      <c r="K89" s="10" t="s">
+      <c r="K90" s="10" t="s">
         <v>877</v>
       </c>
-      <c r="L89" s="114" t="s">
+      <c r="L90" s="114" t="s">
         <v>993</v>
       </c>
     </row>
-    <row r="90" spans="1:12">
-      <c r="A90" s="125" t="s">
-        <v>931</v>
-      </c>
-      <c r="B90" s="10" t="s">
+    <row r="91" spans="1:12">
+      <c r="A91" s="124" t="s">
+        <v>932</v>
+      </c>
+      <c r="B91" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C90" s="127" t="s">
+      <c r="C91" s="126" t="s">
         <v>945</v>
       </c>
-      <c r="D90" s="108" t="s">
+      <c r="D91" s="108" t="s">
         <v>994</v>
       </c>
-      <c r="E90" s="128" t="s">
+      <c r="E91" s="127" t="s">
         <v>996</v>
       </c>
-      <c r="F90" s="113" t="s">
+      <c r="F91" s="113" t="s">
         <v>997</v>
       </c>
-      <c r="G90" s="114" t="s">
+      <c r="G91" s="114" t="s">
         <v>956</v>
       </c>
-      <c r="H90" s="111" t="s">
+      <c r="H91" s="111" t="s">
         <v>970</v>
       </c>
-      <c r="K90" s="10" t="s">
+      <c r="K91" s="10" t="s">
         <v>579</v>
       </c>
-      <c r="L90" s="114" t="s">
+      <c r="L91" s="114" t="s">
         <v>998</v>
       </c>
     </row>
-    <row r="91" spans="1:12">
-      <c r="A91" s="125" t="s">
-        <v>932</v>
-      </c>
-      <c r="B91" s="10" t="s">
+    <row r="92" spans="1:12">
+      <c r="A92" s="124" t="s">
+        <v>933</v>
+      </c>
+      <c r="B92" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C91" s="127" t="s">
+      <c r="C92" s="126" t="s">
         <v>946</v>
       </c>
-      <c r="D91" s="108" t="s">
+      <c r="D92" s="108" t="s">
         <v>702</v>
       </c>
-      <c r="E91" s="128" t="s">
+      <c r="E92" s="127" t="s">
         <v>999</v>
       </c>
-      <c r="F91" s="113" t="s">
+      <c r="F92" s="113" t="s">
         <v>709</v>
       </c>
-      <c r="G91" s="114" t="s">
+      <c r="G92" s="114" t="s">
         <v>957</v>
       </c>
-      <c r="H91" s="111" t="s">
+      <c r="H92" s="111" t="s">
         <v>971</v>
       </c>
-      <c r="K91" s="10" t="s">
+      <c r="K92" s="10" t="s">
         <v>570</v>
       </c>
-      <c r="L91" s="114" t="s">
+      <c r="L92" s="114" t="s">
         <v>1000</v>
       </c>
     </row>
-    <row r="92" spans="1:12">
-      <c r="A92" s="125" t="s">
-        <v>933</v>
-      </c>
-      <c r="B92" s="10" t="s">
+    <row r="93" spans="1:12">
+      <c r="A93" s="124" t="s">
+        <v>934</v>
+      </c>
+      <c r="B93" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C92" s="127" t="s">
+      <c r="C93" s="126" t="s">
         <v>947</v>
       </c>
-      <c r="D92" s="108" t="s">
+      <c r="D93" s="108" t="s">
         <v>444</v>
       </c>
-      <c r="E92" s="128" t="s">
+      <c r="E93" s="127" t="s">
         <v>1008</v>
       </c>
-      <c r="F92" s="113" t="s">
+      <c r="F93" s="113" t="s">
         <v>716</v>
       </c>
-      <c r="G92" s="114" t="s">
+      <c r="G93" s="114" t="s">
         <v>958</v>
       </c>
-      <c r="H92" s="111" t="s">
+      <c r="H93" s="111" t="s">
         <v>972</v>
       </c>
-      <c r="I92" s="10" t="s">
+      <c r="I93" s="10" t="s">
         <v>717</v>
       </c>
-      <c r="L92" s="114" t="s">
+      <c r="L93" s="114" t="s">
         <v>1001</v>
       </c>
     </row>
-    <row r="93" spans="1:12">
-      <c r="A93" s="125" t="s">
-        <v>934</v>
-      </c>
-      <c r="B93" s="10" t="s">
+    <row r="94" spans="1:12">
+      <c r="A94" s="124" t="s">
+        <v>935</v>
+      </c>
+      <c r="B94" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C93" s="127" t="s">
+      <c r="C94" s="126" t="s">
         <v>948</v>
       </c>
-      <c r="D93" s="108" t="s">
+      <c r="D94" s="108" t="s">
         <v>1007</v>
       </c>
-      <c r="E93" s="128" t="s">
+      <c r="E94" s="127" t="s">
         <v>1009</v>
       </c>
-      <c r="F93" s="113" t="s">
+      <c r="F94" s="113" t="s">
         <v>723</v>
       </c>
-      <c r="G93" s="114" t="s">
+      <c r="G94" s="114" t="s">
         <v>959</v>
       </c>
-      <c r="H93" s="111" t="s">
+      <c r="H94" s="111" t="s">
         <v>973</v>
       </c>
-      <c r="I93" s="10" t="s">
+      <c r="I94" s="10" t="s">
         <v>1010</v>
       </c>
-      <c r="L93" s="114" t="s">
+      <c r="L94" s="114" t="s">
         <v>1002</v>
       </c>
     </row>
-    <row r="94" spans="1:12">
-      <c r="A94" s="125" t="s">
-        <v>935</v>
-      </c>
-      <c r="B94" s="10" t="s">
+    <row r="95" spans="1:12">
+      <c r="A95" s="124" t="s">
+        <v>936</v>
+      </c>
+      <c r="B95" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D94" s="109" t="s">
+      <c r="D95" s="109" t="s">
         <v>848</v>
       </c>
-      <c r="E94" s="128" t="s">
+      <c r="E95" s="127" t="s">
         <v>255</v>
       </c>
-      <c r="F94" s="113" t="s">
+      <c r="F95" s="113" t="s">
         <v>1011</v>
       </c>
-      <c r="G94" s="114" t="s">
+      <c r="G95" s="114" t="s">
         <v>960</v>
       </c>
-      <c r="H94" s="111" t="s">
+      <c r="H95" s="111" t="s">
         <v>974</v>
       </c>
-      <c r="I94" s="10" t="s">
+      <c r="I95" s="10" t="s">
         <v>439</v>
       </c>
-      <c r="L94" s="114" t="s">
+      <c r="L95" s="114" t="s">
         <v>1003</v>
       </c>
     </row>
-    <row r="95" spans="1:12">
-      <c r="A95" s="125" t="s">
-        <v>936</v>
-      </c>
-      <c r="B95" s="10" t="s">
+    <row r="96" spans="1:12">
+      <c r="A96" s="124" t="s">
+        <v>937</v>
+      </c>
+      <c r="B96" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C95" s="10" t="s">
+      <c r="C96" s="10" t="s">
         <v>481</v>
       </c>
-      <c r="D95" s="109" t="s">
+      <c r="D96" s="109" t="s">
         <v>708</v>
       </c>
-      <c r="E95" s="128" t="s">
+      <c r="E96" s="127" t="s">
         <v>76</v>
       </c>
-      <c r="F95" s="113" t="s">
+      <c r="F96" s="113" t="s">
         <v>1012</v>
       </c>
-      <c r="G95" s="114" t="s">
+      <c r="G96" s="114" t="s">
         <v>961</v>
       </c>
-      <c r="H95" s="111" t="s">
+      <c r="H96" s="111" t="s">
         <v>975</v>
       </c>
-      <c r="I95" s="10" t="s">
+      <c r="I96" s="10" t="s">
         <v>583</v>
       </c>
-      <c r="K95" s="10" t="s">
+      <c r="K96" s="10" t="s">
         <v>635</v>
       </c>
-      <c r="L95" s="114" t="s">
+      <c r="L96" s="114" t="s">
         <v>1004</v>
       </c>
     </row>
-    <row r="96" spans="1:12">
-      <c r="A96" s="125" t="s">
-        <v>937</v>
-      </c>
-      <c r="B96" s="10" t="s">
+    <row r="97" spans="1:12">
+      <c r="A97" s="124" t="s">
+        <v>938</v>
+      </c>
+      <c r="B97" s="10" t="s">
         <v>298</v>
       </c>
-      <c r="C96" s="10" t="s">
+      <c r="C97" s="10" t="s">
         <v>898</v>
       </c>
-      <c r="D96" s="108" t="s">
+      <c r="D97" s="108" t="s">
         <v>344</v>
       </c>
-      <c r="E96" s="128" t="s">
+      <c r="E97" s="127" t="s">
         <v>223</v>
       </c>
-      <c r="F96" s="113" t="s">
+      <c r="F97" s="143" t="s">
         <v>1013</v>
       </c>
-      <c r="G96" s="114" t="s">
+      <c r="G97" s="114" t="s">
         <v>962</v>
       </c>
-      <c r="H96" s="111" t="s">
+      <c r="H97" s="111" t="s">
         <v>976</v>
       </c>
-      <c r="I96" s="10" t="s">
+      <c r="I97" s="10" t="s">
         <v>474</v>
       </c>
-      <c r="K96" s="10" t="s">
+      <c r="K97" s="10" t="s">
         <v>594</v>
       </c>
-      <c r="L96" s="114" t="s">
+      <c r="L97" s="114" t="s">
         <v>1005</v>
       </c>
     </row>
-    <row r="97" spans="1:12">
-      <c r="A97" s="125" t="s">
-        <v>938</v>
-      </c>
-      <c r="B97" s="10" t="s">
+    <row r="98" spans="1:12">
+      <c r="A98" s="124" t="s">
+        <v>912</v>
+      </c>
+      <c r="B98" s="10" t="s">
         <v>299</v>
       </c>
-      <c r="C97" s="10" t="s">
+      <c r="C98" s="10" t="s">
         <v>902</v>
       </c>
-      <c r="D97" s="108" t="s">
+      <c r="D98" s="108" t="s">
         <v>1014</v>
       </c>
-      <c r="E97" s="128" t="s">
+      <c r="E98" s="127" t="s">
         <v>261</v>
       </c>
-      <c r="F97" s="113" t="s">
+      <c r="F98" s="143" t="s">
         <v>1015</v>
       </c>
-      <c r="G97" s="114" t="s">
+      <c r="G98" s="114" t="s">
         <v>963</v>
       </c>
-      <c r="H97" s="111" t="s">
+      <c r="H98" s="111" t="s">
         <v>977</v>
       </c>
-      <c r="I97" s="10" t="s">
+      <c r="I98" s="10" t="s">
         <v>869</v>
       </c>
-      <c r="L97" s="114" t="s">
+      <c r="L98" s="114" t="s">
         <v>1006</v>
       </c>
     </row>
-    <row r="98" spans="1:12">
-      <c r="A98" s="125" t="s">
-        <v>912</v>
-      </c>
-      <c r="B98" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C98" s="127" t="s">
-        <v>909</v>
-      </c>
-      <c r="D98" s="108" t="s">
-        <v>914</v>
-      </c>
-      <c r="E98" s="10" t="s">
-        <v>915</v>
-      </c>
-      <c r="F98" s="113" t="s">
-        <v>513</v>
-      </c>
-      <c r="G98" s="114" t="s">
-        <v>916</v>
-      </c>
-      <c r="H98" s="111" t="s">
-        <v>919</v>
-      </c>
-      <c r="I98" s="10" t="s">
-        <v>922</v>
-      </c>
-      <c r="K98" s="10" t="s">
-        <v>923</v>
-      </c>
-    </row>
     <row r="99" spans="1:12">
-      <c r="A99" s="126" t="s">
+      <c r="A99" s="125" t="s">
         <v>1070</v>
       </c>
       <c r="B99" s="10" t="s">
@@ -12658,7 +12670,7 @@
       <c r="F99" s="10" t="s">
         <v>1017</v>
       </c>
-      <c r="G99" s="128" t="s">
+      <c r="G99" s="127" t="s">
         <v>255</v>
       </c>
       <c r="H99" s="111" t="s">
@@ -12678,7 +12690,7 @@
       </c>
     </row>
     <row r="100" spans="1:12">
-      <c r="A100" s="126" t="s">
+      <c r="A100" s="125" t="s">
         <v>1071</v>
       </c>
       <c r="B100" s="10" t="s">
@@ -12696,7 +12708,7 @@
       <c r="F100" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="G100" s="128" t="s">
+      <c r="G100" s="127" t="s">
         <v>261</v>
       </c>
       <c r="H100" s="111" t="s">
@@ -12716,7 +12728,7 @@
       </c>
     </row>
     <row r="101" spans="1:12">
-      <c r="A101" s="126" t="s">
+      <c r="A101" s="125" t="s">
         <v>1072</v>
       </c>
       <c r="B101" s="10" t="s">
@@ -12734,7 +12746,7 @@
       <c r="F101" s="113" t="s">
         <v>389</v>
       </c>
-      <c r="G101" s="128" t="s">
+      <c r="G101" s="127" t="s">
         <v>1038</v>
       </c>
       <c r="H101" s="111" t="s">
@@ -12754,7 +12766,7 @@
       </c>
     </row>
     <row r="102" spans="1:12">
-      <c r="A102" s="126" t="s">
+      <c r="A102" s="125" t="s">
         <v>1073</v>
       </c>
       <c r="B102" s="10" t="s">
@@ -12772,7 +12784,7 @@
       <c r="F102" s="113" t="s">
         <v>380</v>
       </c>
-      <c r="G102" s="128" t="s">
+      <c r="G102" s="127" t="s">
         <v>1030</v>
       </c>
       <c r="H102" s="111" t="s">
@@ -12801,7 +12813,7 @@
       <c r="C103" s="10" t="s">
         <v>1077</v>
       </c>
-      <c r="D103" s="108" t="s">
+      <c r="D103" s="143" t="s">
         <v>807</v>
       </c>
       <c r="E103" s="109" t="s">
@@ -12810,7 +12822,7 @@
       <c r="F103" s="10" t="s">
         <v>1079</v>
       </c>
-      <c r="G103" s="128" t="s">
+      <c r="G103" s="127" t="s">
         <v>261</v>
       </c>
       <c r="H103" s="111" t="s">
@@ -12833,7 +12845,7 @@
       <c r="C104" s="10" t="s">
         <v>901</v>
       </c>
-      <c r="D104" s="108" t="s">
+      <c r="D104" s="143" t="s">
         <v>818</v>
       </c>
       <c r="E104" s="109" t="s">
@@ -12842,7 +12854,7 @@
       <c r="F104" s="10" t="s">
         <v>1011</v>
       </c>
-      <c r="G104" s="128" t="s">
+      <c r="G104" s="127" t="s">
         <v>261</v>
       </c>
       <c r="H104" s="111" t="s">
@@ -12872,8 +12884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7498E122-41A9-4336-B180-463F02F789BB}">
   <dimension ref="A1:AI38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K42" sqref="K42"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="V19" sqref="V19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12898,7 +12910,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35">
-      <c r="A1" s="130" t="s">
+      <c r="A1" s="129" t="s">
         <v>30</v>
       </c>
       <c r="B1" s="27" t="s">
@@ -12934,10 +12946,10 @@
       <c r="L1" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="M1" s="140" t="s">
+      <c r="M1" s="139" t="s">
         <v>40</v>
       </c>
-      <c r="V1" s="137" t="s">
+      <c r="V1" s="136" t="s">
         <v>40</v>
       </c>
       <c r="W1" s="55" t="s">
@@ -12978,7 +12990,7 @@
       </c>
     </row>
     <row r="2" spans="1:35">
-      <c r="A2" s="131"/>
+      <c r="A2" s="130"/>
       <c r="B2" s="28"/>
       <c r="C2" s="28"/>
       <c r="D2" s="28"/>
@@ -12990,8 +13002,8 @@
       <c r="J2" s="28"/>
       <c r="K2" s="28"/>
       <c r="L2" s="28"/>
-      <c r="M2" s="131"/>
-      <c r="V2" s="131"/>
+      <c r="M2" s="130"/>
+      <c r="V2" s="130"/>
       <c r="W2" s="28"/>
       <c r="X2" s="28"/>
       <c r="Y2" s="28"/>
@@ -13007,7 +13019,7 @@
       <c r="AI2" s="29"/>
     </row>
     <row r="3" spans="1:35">
-      <c r="A3" s="131"/>
+      <c r="A3" s="130"/>
       <c r="B3" s="28"/>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
@@ -13019,8 +13031,8 @@
       <c r="J3" s="28"/>
       <c r="K3" s="28"/>
       <c r="L3" s="28"/>
-      <c r="M3" s="131"/>
-      <c r="V3" s="131"/>
+      <c r="M3" s="130"/>
+      <c r="V3" s="130"/>
       <c r="W3" s="28"/>
       <c r="X3" s="28"/>
       <c r="Y3" s="28"/>
@@ -13036,7 +13048,7 @@
       <c r="AI3" s="29"/>
     </row>
     <row r="4" spans="1:35">
-      <c r="A4" s="131"/>
+      <c r="A4" s="130"/>
       <c r="B4" s="28"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
@@ -13048,8 +13060,8 @@
       <c r="J4" s="28"/>
       <c r="K4" s="28"/>
       <c r="L4" s="28"/>
-      <c r="M4" s="131"/>
-      <c r="V4" s="131"/>
+      <c r="M4" s="130"/>
+      <c r="V4" s="130"/>
       <c r="W4" s="28"/>
       <c r="X4" s="28"/>
       <c r="Y4" s="28"/>
@@ -13065,7 +13077,7 @@
       <c r="AI4" s="29"/>
     </row>
     <row r="5" spans="1:35">
-      <c r="A5" s="131"/>
+      <c r="A5" s="130"/>
       <c r="B5" s="28"/>
       <c r="C5" s="28"/>
       <c r="D5" s="28"/>
@@ -13077,8 +13089,8 @@
       <c r="J5" s="28"/>
       <c r="K5" s="28"/>
       <c r="L5" s="28"/>
-      <c r="M5" s="131"/>
-      <c r="V5" s="131"/>
+      <c r="M5" s="130"/>
+      <c r="V5" s="130"/>
       <c r="W5" s="28"/>
       <c r="X5" s="28"/>
       <c r="Y5" s="28"/>
@@ -13094,7 +13106,7 @@
       <c r="AI5" s="29"/>
     </row>
     <row r="6" spans="1:35" ht="21" customHeight="1">
-      <c r="A6" s="131"/>
+      <c r="A6" s="130"/>
       <c r="B6" s="28"/>
       <c r="C6" s="28"/>
       <c r="D6" s="28"/>
@@ -13106,7 +13118,7 @@
       <c r="J6" s="28"/>
       <c r="K6" s="28"/>
       <c r="L6" s="28"/>
-      <c r="M6" s="131" t="s">
+      <c r="M6" s="130" t="s">
         <v>1045</v>
       </c>
       <c r="V6" s="36">
@@ -13141,7 +13153,7 @@
       <c r="AI6" s="29"/>
     </row>
     <row r="7" spans="1:35">
-      <c r="A7" s="131"/>
+      <c r="A7" s="130"/>
       <c r="B7" s="28"/>
       <c r="C7" s="28"/>
       <c r="D7" s="28"/>
@@ -13153,7 +13165,7 @@
       <c r="J7" s="28"/>
       <c r="K7" s="28"/>
       <c r="L7" s="28"/>
-      <c r="M7" s="131" t="s">
+      <c r="M7" s="130" t="s">
         <v>1045</v>
       </c>
       <c r="V7" s="43">
@@ -13188,7 +13200,7 @@
       <c r="AI7" s="29"/>
     </row>
     <row r="8" spans="1:35">
-      <c r="A8" s="131"/>
+      <c r="A8" s="130"/>
       <c r="B8" s="28"/>
       <c r="C8" s="28"/>
       <c r="D8" s="28"/>
@@ -13200,16 +13212,16 @@
       <c r="J8" s="28"/>
       <c r="K8" s="28"/>
       <c r="L8" s="28"/>
-      <c r="M8" s="131" t="s">
+      <c r="M8" s="130" t="s">
         <v>1045</v>
       </c>
-      <c r="V8" s="135">
+      <c r="V8" s="134">
         <v>11</v>
       </c>
       <c r="W8" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="X8" s="142">
+      <c r="X8" s="141">
         <v>8.4722222222222227E-2</v>
       </c>
       <c r="Y8" s="52"/>
@@ -13241,7 +13253,7 @@
       <c r="AI8" s="29"/>
     </row>
     <row r="9" spans="1:35">
-      <c r="A9" s="131"/>
+      <c r="A9" s="130"/>
       <c r="B9" s="28"/>
       <c r="C9" s="28"/>
       <c r="D9" s="28"/>
@@ -13253,7 +13265,7 @@
       <c r="J9" s="28"/>
       <c r="K9" s="28"/>
       <c r="L9" s="28"/>
-      <c r="M9" s="131" t="s">
+      <c r="M9" s="130" t="s">
         <v>189</v>
       </c>
       <c r="V9" s="43">
@@ -13288,7 +13300,7 @@
       <c r="AI9" s="29"/>
     </row>
     <row r="10" spans="1:35">
-      <c r="A10" s="131"/>
+      <c r="A10" s="130"/>
       <c r="B10" s="28"/>
       <c r="C10" s="28"/>
       <c r="D10" s="28"/>
@@ -13300,7 +13312,7 @@
       <c r="J10" s="28"/>
       <c r="K10" s="28"/>
       <c r="L10" s="28"/>
-      <c r="M10" s="131" t="s">
+      <c r="M10" s="130" t="s">
         <v>189</v>
       </c>
       <c r="V10" s="36">
@@ -13333,7 +13345,7 @@
       <c r="AI10" s="29"/>
     </row>
     <row r="11" spans="1:35" ht="22.5" customHeight="1">
-      <c r="A11" s="131"/>
+      <c r="A11" s="130"/>
       <c r="B11" s="28"/>
       <c r="C11" s="28"/>
       <c r="D11" s="28"/>
@@ -13345,7 +13357,7 @@
       <c r="J11" s="28"/>
       <c r="K11" s="28"/>
       <c r="L11" s="28"/>
-      <c r="M11" s="131" t="s">
+      <c r="M11" s="130" t="s">
         <v>189</v>
       </c>
       <c r="V11" s="43">
@@ -13378,7 +13390,7 @@
       <c r="AI11" s="29"/>
     </row>
     <row r="12" spans="1:35" ht="18.75" customHeight="1">
-      <c r="A12" s="131"/>
+      <c r="A12" s="130"/>
       <c r="B12" s="28"/>
       <c r="C12" s="28"/>
       <c r="D12" s="28"/>
@@ -13390,7 +13402,7 @@
       <c r="J12" s="28"/>
       <c r="K12" s="28"/>
       <c r="L12" s="28"/>
-      <c r="M12" s="131" t="s">
+      <c r="M12" s="130" t="s">
         <v>189</v>
       </c>
       <c r="V12" s="36">
@@ -13421,7 +13433,7 @@
       <c r="AI12" s="29"/>
     </row>
     <row r="13" spans="1:35">
-      <c r="A13" s="131"/>
+      <c r="A13" s="130"/>
       <c r="B13" s="28"/>
       <c r="C13" s="28"/>
       <c r="D13" s="28"/>
@@ -13433,7 +13445,7 @@
       <c r="J13" s="28"/>
       <c r="K13" s="28"/>
       <c r="L13" s="28"/>
-      <c r="M13" s="131" t="s">
+      <c r="M13" s="130" t="s">
         <v>190</v>
       </c>
       <c r="V13" s="43">
@@ -13464,7 +13476,7 @@
       <c r="AI13" s="29"/>
     </row>
     <row r="14" spans="1:35" ht="18.75" customHeight="1">
-      <c r="A14" s="131"/>
+      <c r="A14" s="130"/>
       <c r="B14" s="28"/>
       <c r="C14" s="28"/>
       <c r="D14" s="28"/>
@@ -13476,7 +13488,7 @@
       <c r="J14" s="28"/>
       <c r="K14" s="41"/>
       <c r="L14" s="28"/>
-      <c r="M14" s="131" t="s">
+      <c r="M14" s="130" t="s">
         <v>192</v>
       </c>
       <c r="V14" s="36">
@@ -13507,7 +13519,7 @@
       <c r="AI14" s="29"/>
     </row>
     <row r="15" spans="1:35">
-      <c r="A15" s="131" t="s">
+      <c r="A15" s="130" t="s">
         <v>1067</v>
       </c>
       <c r="B15" s="28"/>
@@ -13529,7 +13541,7 @@
       <c r="L15" s="28" t="s">
         <v>1064</v>
       </c>
-      <c r="M15" s="131" t="s">
+      <c r="M15" s="130" t="s">
         <v>1063</v>
       </c>
       <c r="V15" s="43">
@@ -13560,7 +13572,7 @@
       <c r="AI15" s="29"/>
     </row>
     <row r="16" spans="1:35">
-      <c r="A16" s="131" t="s">
+      <c r="A16" s="130" t="s">
         <v>1074</v>
       </c>
       <c r="B16" s="28"/>
@@ -13580,7 +13592,7 @@
       <c r="L16" s="28" t="s">
         <v>1065</v>
       </c>
-      <c r="M16" s="131" t="s">
+      <c r="M16" s="130" t="s">
         <v>1062</v>
       </c>
       <c r="V16" s="36">
@@ -13613,7 +13625,7 @@
       <c r="AI16" s="29"/>
     </row>
     <row r="17" spans="1:35">
-      <c r="A17" s="132">
+      <c r="A17" s="131">
         <v>1.1200000000000001</v>
       </c>
       <c r="B17" s="31" t="s">
@@ -13637,7 +13649,7 @@
       <c r="L17" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="M17" s="131" t="s">
+      <c r="M17" s="130" t="s">
         <v>95</v>
       </c>
       <c r="V17" s="43">
@@ -13670,7 +13682,7 @@
       <c r="AI17" s="29"/>
     </row>
     <row r="18" spans="1:35">
-      <c r="A18" s="133">
+      <c r="A18" s="132">
         <v>1.1299999999999999</v>
       </c>
       <c r="B18" s="34" t="s">
@@ -13696,7 +13708,7 @@
       <c r="L18" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="M18" s="131" t="s">
+      <c r="M18" s="130" t="s">
         <v>101</v>
       </c>
       <c r="V18" s="36">
@@ -13765,10 +13777,10 @@
       <c r="L19" s="28" t="s">
         <v>176</v>
       </c>
-      <c r="M19" s="131" t="s">
+      <c r="M19" s="130" t="s">
         <v>175</v>
       </c>
-      <c r="V19" s="138">
+      <c r="V19" s="137">
         <v>47</v>
       </c>
       <c r="W19" s="29" t="s">
@@ -13798,10 +13810,10 @@
       <c r="AI19" s="29"/>
     </row>
     <row r="20" spans="1:35" ht="24.75" customHeight="1">
-      <c r="A20" s="131">
+      <c r="A20" s="130">
         <v>1.19</v>
       </c>
-      <c r="B20" s="129" t="s">
+      <c r="B20" s="128" t="s">
         <v>1054</v>
       </c>
       <c r="C20" s="28"/>
@@ -13823,10 +13835,10 @@
       <c r="L20" s="28" t="s">
         <v>443</v>
       </c>
-      <c r="M20" s="141" t="s">
+      <c r="M20" s="140" t="s">
         <v>1055</v>
       </c>
-      <c r="V20" s="139">
+      <c r="V20" s="138">
         <v>48</v>
       </c>
       <c r="W20" s="58" t="s">
@@ -13856,7 +13868,7 @@
       <c r="AI20" s="29"/>
     </row>
     <row r="21" spans="1:35" ht="18.75" customHeight="1">
-      <c r="A21" s="132">
+      <c r="A21" s="131">
         <v>1.1599999999999999</v>
       </c>
       <c r="B21" s="31" t="s">
@@ -13882,10 +13894,10 @@
       <c r="L21" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="M21" s="131" t="s">
+      <c r="M21" s="130" t="s">
         <v>83</v>
       </c>
-      <c r="V21" s="138">
+      <c r="V21" s="137">
         <v>49</v>
       </c>
       <c r="W21" s="59" t="s">
@@ -13915,7 +13927,7 @@
       <c r="AI21" s="29"/>
     </row>
     <row r="22" spans="1:35">
-      <c r="A22" s="132">
+      <c r="A22" s="131">
         <v>1.18</v>
       </c>
       <c r="B22" s="31" t="s">
@@ -13941,7 +13953,7 @@
       <c r="L22" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="M22" s="131" t="s">
+      <c r="M22" s="130" t="s">
         <v>64</v>
       </c>
       <c r="V22" s="36">
@@ -13978,7 +13990,7 @@
       <c r="AI22" s="29"/>
     </row>
     <row r="23" spans="1:35">
-      <c r="A23" s="131" t="s">
+      <c r="A23" s="130" t="s">
         <v>252</v>
       </c>
       <c r="B23" s="28"/>
@@ -13990,7 +14002,7 @@
         <v>1017</v>
       </c>
       <c r="H23" s="28"/>
-      <c r="I23" s="136">
+      <c r="I23" s="135">
         <v>0.12777777777777777</v>
       </c>
       <c r="J23" s="28" t="s">
@@ -14002,7 +14014,7 @@
       <c r="L23" s="28" t="s">
         <v>1050</v>
       </c>
-      <c r="M23" s="141">
+      <c r="M23" s="140">
         <v>64</v>
       </c>
       <c r="V23" s="43">
@@ -14039,7 +14051,7 @@
       <c r="AI23" s="29"/>
     </row>
     <row r="24" spans="1:35" ht="16.5" customHeight="1">
-      <c r="A24" s="133">
+      <c r="A24" s="132">
         <v>1.17</v>
       </c>
       <c r="B24" s="34" t="s">
@@ -14065,7 +14077,7 @@
       <c r="L24" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="M24" s="131" t="s">
+      <c r="M24" s="130" t="s">
         <v>77</v>
       </c>
       <c r="V24" s="36" t="s">
@@ -14102,7 +14114,7 @@
       <c r="AI24" s="29"/>
     </row>
     <row r="25" spans="1:35" ht="17.25" customHeight="1">
-      <c r="A25" s="133">
+      <c r="A25" s="132">
         <v>1.24</v>
       </c>
       <c r="B25" s="34"/>
@@ -14128,7 +14140,7 @@
       <c r="L25" s="28" t="s">
         <v>151</v>
       </c>
-      <c r="M25" s="131" t="s">
+      <c r="M25" s="130" t="s">
         <v>150</v>
       </c>
       <c r="V25" s="43" t="s">
@@ -14201,10 +14213,10 @@
       <c r="L26" s="28" t="s">
         <v>183</v>
       </c>
-      <c r="M26" s="131" t="s">
+      <c r="M26" s="130" t="s">
         <v>182</v>
       </c>
-      <c r="V26" s="139">
+      <c r="V26" s="138">
         <v>52</v>
       </c>
       <c r="W26" s="58" t="s">
@@ -14232,7 +14244,7 @@
       <c r="AI26" s="29"/>
     </row>
     <row r="27" spans="1:35" ht="18.75" customHeight="1">
-      <c r="A27" s="132">
+      <c r="A27" s="131">
         <v>1.25</v>
       </c>
       <c r="B27" s="31"/>
@@ -14260,10 +14272,10 @@
       <c r="L27" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="M27" s="131" t="s">
+      <c r="M27" s="130" t="s">
         <v>89</v>
       </c>
-      <c r="V27" s="138">
+      <c r="V27" s="137">
         <v>53</v>
       </c>
       <c r="W27" s="59" t="s">
@@ -14291,7 +14303,7 @@
       <c r="AI27" s="29"/>
     </row>
     <row r="28" spans="1:35">
-      <c r="A28" s="131" t="s">
+      <c r="A28" s="130" t="s">
         <v>1057</v>
       </c>
       <c r="B28" s="28"/>
@@ -14300,7 +14312,7 @@
       <c r="E28" s="28"/>
       <c r="F28" s="28"/>
       <c r="H28" s="28"/>
-      <c r="I28" s="136">
+      <c r="I28" s="135">
         <v>0.12847222222222221</v>
       </c>
       <c r="J28" s="28" t="s">
@@ -14312,10 +14324,10 @@
       <c r="L28" s="28" t="s">
         <v>1051</v>
       </c>
-      <c r="M28" s="141">
+      <c r="M28" s="140">
         <v>65</v>
       </c>
-      <c r="V28" s="138">
+      <c r="V28" s="137">
         <v>54</v>
       </c>
       <c r="W28" s="58" t="s">
@@ -14343,7 +14355,7 @@
       <c r="AI28" s="29"/>
     </row>
     <row r="29" spans="1:35" ht="17.25" customHeight="1">
-      <c r="A29" s="131" t="s">
+      <c r="A29" s="130" t="s">
         <v>1058</v>
       </c>
       <c r="B29" s="28"/>
@@ -14355,10 +14367,10 @@
         <v>54</v>
       </c>
       <c r="H29" s="28"/>
-      <c r="I29" s="136">
+      <c r="I29" s="135">
         <v>0.13333333333333333</v>
       </c>
-      <c r="J29" s="136">
+      <c r="J29" s="135">
         <v>8.4027777777777785E-2</v>
       </c>
       <c r="K29" s="104" t="s">
@@ -14367,10 +14379,10 @@
       <c r="L29" s="28" t="s">
         <v>1052</v>
       </c>
-      <c r="M29" s="141">
+      <c r="M29" s="140">
         <v>66</v>
       </c>
-      <c r="V29" s="138">
+      <c r="V29" s="137">
         <v>55</v>
       </c>
       <c r="W29" s="59" t="s">
@@ -14398,7 +14410,7 @@
       <c r="AI29" s="29"/>
     </row>
     <row r="30" spans="1:35">
-      <c r="A30" s="131" t="s">
+      <c r="A30" s="130" t="s">
         <v>1059</v>
       </c>
       <c r="B30" s="28"/>
@@ -14410,10 +14422,10 @@
         <v>50</v>
       </c>
       <c r="H30" s="28"/>
-      <c r="I30" s="136">
+      <c r="I30" s="135">
         <v>0.13402777777777777</v>
       </c>
-      <c r="J30" s="136">
+      <c r="J30" s="135">
         <v>8.4722222222222227E-2</v>
       </c>
       <c r="K30" s="104" t="s">
@@ -14422,10 +14434,10 @@
       <c r="L30" s="28" t="s">
         <v>1053</v>
       </c>
-      <c r="M30" s="141">
+      <c r="M30" s="140">
         <v>67</v>
       </c>
-      <c r="V30" s="138">
+      <c r="V30" s="137">
         <v>56</v>
       </c>
       <c r="W30" s="58" t="s">
@@ -14453,7 +14465,7 @@
       <c r="AI30" s="29"/>
     </row>
     <row r="31" spans="1:35" ht="18.75" customHeight="1">
-      <c r="A31" s="131" t="s">
+      <c r="A31" s="130" t="s">
         <v>231</v>
       </c>
       <c r="B31" s="28"/>
@@ -14463,10 +14475,10 @@
       <c r="F31" s="28"/>
       <c r="G31" s="28"/>
       <c r="H31" s="28"/>
-      <c r="I31" s="136">
+      <c r="I31" s="135">
         <v>0.13472222222222222</v>
       </c>
-      <c r="J31" s="136">
+      <c r="J31" s="135">
         <v>8.5416666666666669E-2</v>
       </c>
       <c r="K31" s="104" t="s">
@@ -14475,10 +14487,10 @@
       <c r="L31" s="28" t="s">
         <v>230</v>
       </c>
-      <c r="M31" s="141">
+      <c r="M31" s="140">
         <v>26</v>
       </c>
-      <c r="V31" s="138">
+      <c r="V31" s="137">
         <v>57</v>
       </c>
       <c r="W31" s="59" t="s">
@@ -14506,7 +14518,7 @@
       <c r="AI31" s="29"/>
     </row>
     <row r="32" spans="1:35">
-      <c r="A32" s="134">
+      <c r="A32" s="133">
         <v>1.2</v>
       </c>
       <c r="B32" s="48" t="s">
@@ -14531,10 +14543,10 @@
       <c r="L32" s="28" t="s">
         <v>164</v>
       </c>
-      <c r="M32" s="131">
-        <v>1</v>
-      </c>
-      <c r="V32" s="138">
+      <c r="M32" s="130" t="s">
+        <v>1082</v>
+      </c>
+      <c r="V32" s="137">
         <v>58</v>
       </c>
       <c r="W32" s="58" t="s">
@@ -14562,7 +14574,7 @@
       <c r="AI32" s="29"/>
     </row>
     <row r="33" spans="1:35" ht="17.25" customHeight="1">
-      <c r="A33" s="135">
+      <c r="A33" s="134">
         <v>1.3</v>
       </c>
       <c r="B33" s="52" t="s">
@@ -14588,10 +14600,10 @@
       <c r="L33" s="28" t="s">
         <v>141</v>
       </c>
-      <c r="M33" s="131">
-        <v>0</v>
-      </c>
-      <c r="V33" s="138">
+      <c r="M33" s="130" t="s">
+        <v>1083</v>
+      </c>
+      <c r="V33" s="137">
         <v>59</v>
       </c>
       <c r="W33" s="59" t="s">
@@ -14619,7 +14631,7 @@
       <c r="AI33" s="29"/>
     </row>
     <row r="34" spans="1:35" ht="18" customHeight="1">
-      <c r="A34" s="133" t="s">
+      <c r="A34" s="132" t="s">
         <v>207</v>
       </c>
       <c r="B34" s="34" t="s">
@@ -14655,7 +14667,7 @@
       <c r="L34" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="M34" s="131" t="s">
+      <c r="M34" s="130" t="s">
         <v>70</v>
       </c>
       <c r="V34" s="36" t="s">
@@ -14686,7 +14698,7 @@
       <c r="AI34" s="29"/>
     </row>
     <row r="35" spans="1:35" ht="17.25" customHeight="1">
-      <c r="A35" s="132" t="s">
+      <c r="A35" s="131" t="s">
         <v>205</v>
       </c>
       <c r="B35" s="31" t="s">
@@ -14722,7 +14734,7 @@
       <c r="L35" s="28" t="s">
         <v>158</v>
       </c>
-      <c r="M35" s="131" t="s">
+      <c r="M35" s="130" t="s">
         <v>157</v>
       </c>
       <c r="V35" s="43" t="s">
@@ -14753,7 +14765,7 @@
       <c r="AI35" s="29"/>
     </row>
     <row r="36" spans="1:35" ht="15.75" customHeight="1">
-      <c r="A36" s="133">
+      <c r="A36" s="132">
         <v>1.31</v>
       </c>
       <c r="B36" s="34"/>
@@ -14779,10 +14791,10 @@
       <c r="L36" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="M36" s="131" t="s">
+      <c r="M36" s="130" t="s">
         <v>108</v>
       </c>
-      <c r="V36" s="138">
+      <c r="V36" s="137">
         <v>62</v>
       </c>
       <c r="W36" s="29" t="s">
@@ -14812,7 +14824,7 @@
       <c r="AI36" s="29"/>
     </row>
     <row r="37" spans="1:35" ht="18" customHeight="1">
-      <c r="A37" s="131"/>
+      <c r="A37" s="130"/>
       <c r="B37" s="28"/>
       <c r="C37" s="28"/>
       <c r="D37" s="28"/>
@@ -14824,10 +14836,10 @@
       <c r="J37" s="28"/>
       <c r="K37" s="28"/>
       <c r="L37" s="28"/>
-      <c r="M37" s="131" t="s">
+      <c r="M37" s="130" t="s">
         <v>191</v>
       </c>
-      <c r="V37" s="138">
+      <c r="V37" s="137">
         <v>63</v>
       </c>
       <c r="W37" s="29" t="s">

</xml_diff>